<commit_message>
SIT in VM (10-04-2023)
SIT in VM (10-04-2023)

Co-Authored-By: kokyu9807 <125843958+kokyu9807@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Project_Notebook.xlsx
+++ b/Project_Notebook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dfa8e453c68a9915/Documents/UiPath/SCC - Kuantan/GitHub/Auto-Generate-LE-Weekly-Report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SCC-IT\Documents\UiPath\SCC-Kuantan\GitHub\Auto-Generate-LE-Weekly-Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="465" documentId="13_ncr:1_{9C61E94F-7D39-409B-9B4B-F937306AB8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CEC03D8-EADA-4A40-8AAC-14A53A9B041E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978567F3-E4FD-4D80-B6C3-2AD73910CDCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Scratchpad" sheetId="6" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="File" sheetId="5" r:id="rId5"/>
     <sheet name="Config" sheetId="8" r:id="rId6"/>
     <sheet name="Access" sheetId="7" r:id="rId7"/>
-    <sheet name="About the Project Notebook" sheetId="2" r:id="rId8"/>
+    <sheet name="Access (2)" sheetId="9" r:id="rId8"/>
+    <sheet name="About the Project Notebook" sheetId="2" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_A1">Scratchpad!$A$1</definedName>
@@ -44,10 +45,12 @@
     <definedName name="FirstName">Text!$B$15</definedName>
     <definedName name="Folder">File!$B$11</definedName>
     <definedName name="FullFileName_Input">File!$B$6</definedName>
-    <definedName name="ID">Access!$B$10</definedName>
     <definedName name="Int">Number!$B$6</definedName>
+    <definedName name="KB" localSheetId="7">'Access (2)'!$B$15</definedName>
     <definedName name="KB">Access!$B$15</definedName>
+    <definedName name="KT" localSheetId="7">'Access (2)'!$B$22</definedName>
     <definedName name="KT">Access!$B$22</definedName>
+    <definedName name="KU" localSheetId="7">'Access (2)'!$B$1</definedName>
     <definedName name="KU">Access!$B$1</definedName>
     <definedName name="LastBzDayFri">Date!$B$20</definedName>
     <definedName name="LastBzDayThu">Date!$C$20</definedName>
@@ -57,43 +60,76 @@
     <definedName name="LastWeekFriday">Date!#REF!</definedName>
     <definedName name="LastWeekMonday">Date!$B$14</definedName>
     <definedName name="LastWeekSunday">Date!#REF!</definedName>
+    <definedName name="LE_KB_CREDENTIAL" localSheetId="7">'Access (2)'!$B$20</definedName>
     <definedName name="LE_KB_CREDENTIAL">Access!$B$20</definedName>
+    <definedName name="LE_KB_ID" localSheetId="7">'Access (2)'!$B$17</definedName>
     <definedName name="LE_KB_ID">Access!$B$17</definedName>
+    <definedName name="LE_KB_PWD" localSheetId="7">'Access (2)'!$B$19</definedName>
     <definedName name="LE_KB_PWD">Access!$B$19</definedName>
+    <definedName name="LE_KB_URL" localSheetId="7">'Access (2)'!$B$16</definedName>
     <definedName name="LE_KB_URL">Access!$B$16</definedName>
+    <definedName name="LE_KB_USERNAME" localSheetId="7">'Access (2)'!$B$18</definedName>
     <definedName name="LE_KB_USERNAME">Access!$B$18</definedName>
+    <definedName name="LE_KT_CREDENTIAL" localSheetId="7">'Access (2)'!$B$27</definedName>
     <definedName name="LE_KT_CREDENTIAL">Access!$B$27</definedName>
+    <definedName name="LE_KT_ID" localSheetId="7">'Access (2)'!$B$24</definedName>
     <definedName name="LE_KT_ID">Access!$B$24</definedName>
+    <definedName name="LE_KT_PWD" localSheetId="7">'Access (2)'!$B$26</definedName>
     <definedName name="LE_KT_PWD">Access!$B$26</definedName>
+    <definedName name="LE_KT_URL" localSheetId="7">'Access (2)'!#REF!</definedName>
     <definedName name="LE_KT_URL">Access!#REF!</definedName>
+    <definedName name="LE_KT_USERNAME" localSheetId="7">'Access (2)'!$B$25</definedName>
     <definedName name="LE_KT_USERNAME">Access!$B$25</definedName>
+    <definedName name="LE_KU_CREDENTIAL" localSheetId="7">'Access (2)'!$B$6</definedName>
     <definedName name="LE_KU_CREDENTIAL">Access!$B$6</definedName>
+    <definedName name="LE_KU_ID" localSheetId="7">'Access (2)'!$B$3</definedName>
     <definedName name="LE_KU_ID">Access!$B$3</definedName>
+    <definedName name="LE_KU_PWD" localSheetId="7">'Access (2)'!$B$5</definedName>
     <definedName name="LE_KU_PWD">Access!$B$5</definedName>
+    <definedName name="LE_KU_URL" localSheetId="7">'Access (2)'!$B$2</definedName>
     <definedName name="LE_KU_URL">Access!$B$2</definedName>
+    <definedName name="LE_KU_USERNAME" localSheetId="7">'Access (2)'!$B$4</definedName>
     <definedName name="LE_KU_USERNAME">Access!$B$4</definedName>
+    <definedName name="LE_MK_CREDENTIAL" localSheetId="7">'Access (2)'!$B$13</definedName>
     <definedName name="LE_MK_CREDENTIAL">Access!$B$13</definedName>
+    <definedName name="LE_MK_ID" localSheetId="7">'Access (2)'!$B$10</definedName>
     <definedName name="LE_MK_ID">Access!$B$10</definedName>
+    <definedName name="LE_MK_PWD" localSheetId="7">'Access (2)'!$B$12</definedName>
     <definedName name="LE_MK_PWD">Access!$B$12</definedName>
+    <definedName name="LE_MK_URL" localSheetId="7">'Access (2)'!$B$9</definedName>
     <definedName name="LE_MK_URL">Access!$B$9</definedName>
+    <definedName name="LE_MK_USERNAME" localSheetId="7">'Access (2)'!$B$11</definedName>
     <definedName name="LE_MK_USERNAME">Access!$B$11</definedName>
-    <definedName name="LE_PC_CREDENTIAL">Access!$B$34</definedName>
-    <definedName name="LE_PC_ID">Access!$B$31</definedName>
-    <definedName name="LE_PC_PWD">Access!$B$33</definedName>
-    <definedName name="LE_PC_URL">Access!$B$30</definedName>
-    <definedName name="LE_PC_URL_LOCAL">Access!$C$30</definedName>
-    <definedName name="LE_PC_USERNAME">Access!$B$32</definedName>
-    <definedName name="LE_SB_CREDENTIAL">Access!$B$41</definedName>
-    <definedName name="LE_SB_ID">Access!$B$38</definedName>
-    <definedName name="LE_SB_PWD">Access!$B$40</definedName>
-    <definedName name="LE_SB_URL">Access!$B$37</definedName>
-    <definedName name="LE_SB_USERNAME">Access!$B$39</definedName>
+    <definedName name="LE_PC_CREDENTIAL" localSheetId="7">'Access (2)'!$B$34</definedName>
+    <definedName name="LE_PC_CREDENTIAL">Access!#REF!</definedName>
+    <definedName name="LE_PC_ID" localSheetId="7">'Access (2)'!$B$31</definedName>
+    <definedName name="LE_PC_ID">Access!#REF!</definedName>
+    <definedName name="LE_PC_PWD" localSheetId="7">'Access (2)'!$B$33</definedName>
+    <definedName name="LE_PC_PWD">Access!#REF!</definedName>
+    <definedName name="LE_PC_URL" localSheetId="7">'Access (2)'!$B$30</definedName>
+    <definedName name="LE_PC_URL">Access!#REF!</definedName>
+    <definedName name="LE_PC_URL_LOCAL" localSheetId="7">'Access (2)'!$C$30</definedName>
+    <definedName name="LE_PC_URL_LOCAL">Access!#REF!</definedName>
+    <definedName name="LE_PC_USERNAME" localSheetId="7">'Access (2)'!$B$32</definedName>
+    <definedName name="LE_PC_USERNAME">Access!#REF!</definedName>
+    <definedName name="LE_SB_CREDENTIAL" localSheetId="7">'Access (2)'!$B$41</definedName>
+    <definedName name="LE_SB_CREDENTIAL">Access!#REF!</definedName>
+    <definedName name="LE_SB_ID" localSheetId="7">'Access (2)'!$B$38</definedName>
+    <definedName name="LE_SB_ID">Access!#REF!</definedName>
+    <definedName name="LE_SB_PWD" localSheetId="7">'Access (2)'!$B$40</definedName>
+    <definedName name="LE_SB_PWD">Access!#REF!</definedName>
+    <definedName name="LE_SB_URL" localSheetId="7">'Access (2)'!$B$37</definedName>
+    <definedName name="LE_SB_URL">Access!#REF!</definedName>
+    <definedName name="LE_SB_USERNAME" localSheetId="7">'Access (2)'!$B$39</definedName>
+    <definedName name="LE_SB_USERNAME">Access!#REF!</definedName>
     <definedName name="Length">Text!$B$6</definedName>
     <definedName name="LowerCase">Text!$B$8</definedName>
+    <definedName name="MK" localSheetId="7">'Access (2)'!$B$8</definedName>
     <definedName name="MK">Access!$B$8</definedName>
     <definedName name="Number_Input">Number!$B$4</definedName>
     <definedName name="NumberText_Input">Number!$B$11</definedName>
-    <definedName name="PC">Access!$B$29</definedName>
+    <definedName name="PC" localSheetId="7">'Access (2)'!$B$29</definedName>
+    <definedName name="PC">Access!#REF!</definedName>
     <definedName name="preferred_date_format">Date!$B$6</definedName>
     <definedName name="Process_Folder">Config!$B$1</definedName>
     <definedName name="ReformattedDate">Date!$B$37</definedName>
@@ -133,7 +169,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="145">
   <si>
     <t>Last month's dates (First and Last)</t>
   </si>
@@ -568,6 +604,9 @@
   </si>
   <si>
     <t>reports/reportform.aspx?qs=/SNDReports/UMM%20Goods%20Returned%20Report</t>
+  </si>
+  <si>
+    <t>eric.tan@sccsb.com.my</t>
   </si>
 </sst>
 </file>
@@ -1110,7 +1149,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1244,6 +1283,9 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1461,10 +1503,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF8D5779-502D-0378-BAF0-00F11A69086C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D202501-C8DA-4793-8648-7A720A3C3368}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1480,7 +1522,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8450580" y="6426282"/>
+          <a:off x="9113520" y="6365322"/>
           <a:ext cx="2812123" cy="1887367"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1584,10 +1626,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1891,10 +1929,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.77734375" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1906,35 +1944,35 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="15.77734375" style="27" customWidth="1"/>
+    <col min="2" max="8" width="15.7109375" style="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-    </row>
-    <row r="2" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60" t="s">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+    </row>
+    <row r="2" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -1946,7 +1984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -1954,7 +1992,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -1962,7 +2000,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -1971,7 +2009,7 @@
         <v>05/04/2023</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -1980,7 +2018,7 @@
         <v>03/04/2023</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1989,7 +2027,7 @@
         <v>20230410</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1998,7 +2036,7 @@
         <v>10/04/2023</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -2031,7 +2069,7 @@
         <v>10/04/2023</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>121</v>
       </c>
@@ -2064,7 +2102,7 @@
         <v>09/04/2023</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -2077,7 +2115,7 @@
         <v>31/03/2023</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -2090,11 +2128,11 @@
         <v>28/04/2023</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" s="30"/>
       <c r="C17" s="30"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
         <v>106</v>
       </c>
@@ -2105,7 +2143,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>124</v>
       </c>
@@ -2118,7 +2156,7 @@
         <v>02/04/2023</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>125</v>
       </c>
@@ -2131,36 +2169,36 @@
         <v>06/04/2023</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="30"/>
       <c r="C21" s="30"/>
     </row>
-    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="56" t="s">
+    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="58"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="59"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D24" s="31"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="54" t="s">
+      <c r="B25" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="55"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C25" s="55"/>
+      <c r="D25" s="56"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>22</v>
       </c>
@@ -2174,7 +2212,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>23</v>
       </c>
@@ -2183,13 +2221,13 @@
       </c>
       <c r="D27" s="31"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>20</v>
       </c>
       <c r="D28" s="31"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>27</v>
       </c>
@@ -2206,7 +2244,7 @@
         <v>12月31</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>28</v>
       </c>
@@ -2216,7 +2254,7 @@
       </c>
       <c r="D30" s="31"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>29</v>
       </c>
@@ -2226,7 +2264,7 @@
       </c>
       <c r="D31" s="31"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>30</v>
       </c>
@@ -2240,7 +2278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>31</v>
       </c>
@@ -2250,7 +2288,7 @@
       </c>
       <c r="D33" s="31"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>32</v>
       </c>
@@ -2260,13 +2298,13 @@
       </c>
       <c r="D34" s="31"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D35" s="31"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>84</v>
       </c>
@@ -2276,7 +2314,7 @@
       </c>
       <c r="D36" s="31"/>
     </row>
-    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>24</v>
       </c>
@@ -2307,36 +2345,36 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60" t="s">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+    </row>
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -2356,7 +2394,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2378,7 +2416,7 @@
         <v>C.</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2397,7 +2435,7 @@
         <v>C. Doe</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -2416,7 +2454,7 @@
         <v>John C.</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -2435,7 +2473,7 @@
         <v>Doe</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>63</v>
       </c>
@@ -2444,7 +2482,7 @@
         <v>John C. Doe</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -2455,7 +2493,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -2466,7 +2504,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -2478,7 +2516,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -2490,12 +2528,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -2507,7 +2545,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -2519,7 +2557,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>63</v>
       </c>
@@ -2542,37 +2580,37 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.77734375" customWidth="1"/>
-    <col min="4" max="4" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="59"/>
+      <c r="B1" s="60"/>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60" t="s">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="60"/>
+      <c r="B2" s="61"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -2580,7 +2618,7 @@
         <v>3.1415929999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -2589,7 +2627,7 @@
         <v>3.1415929999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -2598,7 +2636,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -2607,20 +2645,20 @@
         <v>3.14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="56" t="s">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="58"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="59"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>19</v>
       </c>
@@ -2628,7 +2666,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>33</v>
       </c>
@@ -2637,7 +2675,7 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>34</v>
       </c>
@@ -2645,13 +2683,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>35</v>
       </c>
@@ -2679,48 +2717,48 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="4" width="15.21875" customWidth="1"/>
+    <col min="3" max="4" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="59"/>
+      <c r="B1" s="60"/>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60" t="s">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="60"/>
+      <c r="B2" s="61"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
     </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="56" t="s">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="58"/>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="59"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
@@ -2728,13 +2766,13 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>39</v>
       </c>
@@ -2743,7 +2781,7 @@
         <v>Untitled Document.docx</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>41</v>
       </c>
@@ -2752,7 +2790,7 @@
         <v>docx</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>40</v>
       </c>
@@ -2761,7 +2799,7 @@
         <v>Untitled Document</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>55</v>
       </c>
@@ -2770,7 +2808,7 @@
         <v>C:\temp\</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -2791,19 +2829,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D25349-4B39-4221-90B0-AC4514B6ED0A}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" style="29" customWidth="1"/>
-    <col min="2" max="2" width="80.5546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" style="29" customWidth="1"/>
+    <col min="2" max="2" width="80.5703125" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>112</v>
       </c>
@@ -2811,7 +2849,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>118</v>
       </c>
@@ -2819,23 +2857,23 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="28" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="54" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>116</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>142</v>
       </c>
@@ -2843,32 +2881,45 @@
         <v>143</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="28" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="28" t="s">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{9080513A-37F3-4ABB-8407-050FD5A64DCB}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B29D1A0-C4ED-4248-BED6-5082308831E6}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" style="26" customWidth="1"/>
-    <col min="2" max="2" width="41.33203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5546875" style="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.77734375" style="50" customWidth="1"/>
-    <col min="5" max="5" width="50.33203125" style="40" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="40"/>
+    <col min="1" max="1" width="15.7109375" style="26" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.7109375" style="50" customWidth="1"/>
+    <col min="5" max="5" width="50.28515625" style="40" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>106</v>
       </c>
@@ -2877,7 +2928,7 @@
       </c>
       <c r="D1" s="53"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>89</v>
       </c>
@@ -2885,7 +2936,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>87</v>
       </c>
@@ -2893,7 +2944,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>88</v>
       </c>
@@ -2901,7 +2952,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>91</v>
       </c>
@@ -2910,12 +2961,12 @@
       </c>
       <c r="D5" s="51"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="44" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>106</v>
       </c>
@@ -2924,7 +2975,7 @@
       </c>
       <c r="D8" s="53"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>89</v>
       </c>
@@ -2932,7 +2983,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>87</v>
       </c>
@@ -2940,7 +2991,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>88</v>
       </c>
@@ -2948,7 +2999,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>91</v>
       </c>
@@ -2956,12 +3007,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="44" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>106</v>
       </c>
@@ -2970,7 +3021,7 @@
       </c>
       <c r="D15" s="53"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>89</v>
       </c>
@@ -2978,7 +3029,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
         <v>87</v>
       </c>
@@ -2986,7 +3037,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
         <v>88</v>
       </c>
@@ -2994,7 +3045,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
         <v>91</v>
       </c>
@@ -3002,12 +3053,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="47" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
         <v>106</v>
       </c>
@@ -3016,7 +3067,7 @@
       </c>
       <c r="D22" s="53"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>89</v>
       </c>
@@ -3026,7 +3077,7 @@
       <c r="C23" s="49"/>
       <c r="D23" s="52"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
         <v>87</v>
       </c>
@@ -3034,7 +3085,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
         <v>88</v>
       </c>
@@ -3042,7 +3093,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
         <v>91</v>
       </c>
@@ -3051,159 +3102,382 @@
       </c>
       <c r="D26" s="51"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="44" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="B29" s="41" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="B30" s="48" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" s="38" t="s">
-        <v>95</v>
-      </c>
-      <c r="D30" s="51" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31" s="43">
-        <v>71600223</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="B32" s="43" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="B33" s="43" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="44" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="B36" s="41" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="B37" s="45" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="B38" s="43" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" s="43" t="s">
-        <v>104</v>
-      </c>
-      <c r="D39" s="51" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="B40" s="43" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="44" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="B48" s="41" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="B49" s="45" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="B50" s="43" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" s="43" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="B52" s="43" t="s">
-        <v>104</v>
-      </c>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="41"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="45"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B16" r:id="rId1" xr:uid="{1EC1A304-61A3-46EC-8DE3-72735D1D87B9}"/>
-    <hyperlink ref="B30" r:id="rId2" xr:uid="{E1719E05-38A6-43C4-AF5F-A253115D11CF}"/>
-    <hyperlink ref="C30" r:id="rId3" xr:uid="{38C0FA9B-05AA-45E1-8A5C-96DEFFF04CB6}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{1BD0729C-9149-4664-845E-1EB8AD0373E2}"/>
-    <hyperlink ref="B37" r:id="rId5" xr:uid="{DB1BD3A6-5704-4E2D-8025-BC9C9FFA5742}"/>
-    <hyperlink ref="B9" r:id="rId6" xr:uid="{8AC85A88-86DC-42DE-A409-97861D058B75}"/>
-    <hyperlink ref="B49" r:id="rId7" xr:uid="{2F4C1523-8683-4AC0-9541-3C0FE8D14C11}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{1BD0729C-9149-4664-845E-1EB8AD0373E2}"/>
+    <hyperlink ref="B9" r:id="rId3" xr:uid="{8AC85A88-86DC-42DE-A409-97861D058B75}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72C5A992-EEE8-4D34-9600-D196F5D830BD}">
+  <dimension ref="A1:D52"/>
+  <sheetViews>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" style="26" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" style="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.7109375" style="50" customWidth="1"/>
+    <col min="5" max="5" width="50.28515625" style="40" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="40"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="53"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="51"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="44" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="53"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="44" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="53"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="43" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="46" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="47" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="53"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" s="49"/>
+      <c r="D23" s="52"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="43" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="43" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="51"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="44" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="41" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="51" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" s="43">
+        <v>71600223</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="43" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="43" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="44" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" s="41" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" s="45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="43" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" s="51" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" s="43" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="44" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B48" s="41" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" s="45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="43" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="43" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" s="43" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B16" r:id="rId1" xr:uid="{D43FD02D-8790-4C2F-8D40-7C4518D0BDA4}"/>
+    <hyperlink ref="B30" r:id="rId2" xr:uid="{CEFD86C0-219A-49B1-93DF-1F7DFC7A7F69}"/>
+    <hyperlink ref="C30" r:id="rId3" xr:uid="{1C4F0EFD-B2F6-40D0-8932-49FBE7BC73CB}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{8DA2F361-99B4-4E59-8D22-40537CEE6CEF}"/>
+    <hyperlink ref="B37" r:id="rId5" xr:uid="{4C45FE0D-0413-45DE-B9BB-766DDC10ABDA}"/>
+    <hyperlink ref="B9" r:id="rId6" xr:uid="{2BDF0F0E-B8CD-45B8-9985-A56F880AF2CF}"/>
+    <hyperlink ref="B49" r:id="rId7" xr:uid="{43F2D25B-ECF5-4DAB-B19A-44F94EA336F3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
@@ -3211,120 +3485,120 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88115396-113A-4E92-ABEE-648E1977C738}">
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="165.5546875" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="165.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19"/>
     </row>
-    <row r="2" spans="1:5" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="D4" s="16"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>70</v>
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>74</v>
       </c>

</xml_diff>

<commit_message>
Commit in VM (17-04-2023)
Commit in VM (17-04-2023)
</commit_message>
<xml_diff>
--- a/Project_Notebook.xlsx
+++ b/Project_Notebook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SCC-IT\Documents\UiPath\SCC-Kuantan\GitHub\Auto-Generate-LE-Weekly-Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E0B5C7-4A8B-4DD7-8E85-32741420F0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52234FB9-6F73-4070-A4D0-D4BAFC7C552B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9024" firstSheet="1" activeTab="6" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Scratchpad" sheetId="6" r:id="rId1"/>
@@ -1188,7 +1188,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1371,6 +1371,9 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1394,6 +1397,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -1965,10 +1971,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1983,32 +1989,32 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="15.7109375" style="26" customWidth="1"/>
+    <col min="2" max="8" width="15.6640625" style="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-    </row>
-    <row r="2" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+    </row>
+    <row r="2" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="77" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
@@ -2020,7 +2026,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -2028,7 +2034,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -2036,7 +2042,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -2045,7 +2051,7 @@
         <v>07/04/2023</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -2054,7 +2060,7 @@
         <v>05/04/2023</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2063,7 +2069,7 @@
         <v>20230412</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -2072,7 +2078,7 @@
         <v>12/04/2023</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>119</v>
       </c>
@@ -2105,7 +2111,7 @@
         <v>12/04/2023</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>120</v>
       </c>
@@ -2138,7 +2144,7 @@
         <v>09/04/2023</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -2151,7 +2157,7 @@
         <v>31/03/2023</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -2164,11 +2170,11 @@
         <v>28/04/2023</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="35" t="s">
         <v>105</v>
       </c>
@@ -2179,7 +2185,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>142</v>
       </c>
@@ -2192,7 +2198,7 @@
         <v>04/04/2023</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>123</v>
       </c>
@@ -2205,36 +2211,36 @@
         <v>08/04/2023</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
     </row>
-    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="72" t="s">
+    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="73"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="74"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="75"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D24" s="30"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="70" t="s">
+      <c r="B25" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="70"/>
-      <c r="D25" s="71"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="71"/>
+      <c r="D25" s="72"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>22</v>
       </c>
@@ -2248,7 +2254,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>23</v>
       </c>
@@ -2257,13 +2263,13 @@
       </c>
       <c r="D27" s="30"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>20</v>
       </c>
       <c r="D28" s="30"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>27</v>
       </c>
@@ -2280,7 +2286,7 @@
         <v>12月31</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>28</v>
       </c>
@@ -2290,7 +2296,7 @@
       </c>
       <c r="D30" s="30"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>29</v>
       </c>
@@ -2300,7 +2306,7 @@
       </c>
       <c r="D31" s="30"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>30</v>
       </c>
@@ -2314,7 +2320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>31</v>
       </c>
@@ -2324,7 +2330,7 @@
       </c>
       <c r="D33" s="30"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>32</v>
       </c>
@@ -2334,13 +2340,13 @@
       </c>
       <c r="D34" s="30"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D35" s="30"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="25" t="s">
         <v>84</v>
       </c>
@@ -2350,7 +2356,7 @@
       </c>
       <c r="D36" s="30"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
         <v>24</v>
       </c>
@@ -2381,36 +2387,36 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+    </row>
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -2430,7 +2436,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2452,7 +2458,7 @@
         <v>C.</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2471,7 +2477,7 @@
         <v>C. Doe</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -2490,7 +2496,7 @@
         <v>John C.</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -2509,7 +2515,7 @@
         <v>Doe</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>63</v>
       </c>
@@ -2518,7 +2524,7 @@
         <v>John C. Doe</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -2529,7 +2535,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -2540,7 +2546,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -2552,7 +2558,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -2564,12 +2570,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -2581,7 +2587,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -2593,7 +2599,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>63</v>
       </c>
@@ -2616,37 +2622,37 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="75"/>
+      <c r="B1" s="76"/>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="76"/>
+      <c r="B2" s="77"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -2654,7 +2660,7 @@
         <v>3.1415929999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -2663,7 +2669,7 @@
         <v>3.1415929999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -2672,7 +2678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -2681,20 +2687,20 @@
         <v>3.14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="72" t="s">
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="74"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="75"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>19</v>
       </c>
@@ -2702,7 +2708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>33</v>
       </c>
@@ -2711,7 +2717,7 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>34</v>
       </c>
@@ -2719,13 +2725,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>35</v>
       </c>
@@ -2753,48 +2759,48 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="4" width="15.28515625" customWidth="1"/>
+    <col min="3" max="4" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="76" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="75"/>
+      <c r="B1" s="76"/>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="77" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="76"/>
+      <c r="B2" s="77"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="72" t="s">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="74"/>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="75"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>39</v>
       </c>
@@ -2802,13 +2808,13 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>39</v>
       </c>
@@ -2817,7 +2823,7 @@
         <v>Untitled Document.docx</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>41</v>
       </c>
@@ -2826,7 +2832,7 @@
         <v>docx</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>40</v>
       </c>
@@ -2835,7 +2841,7 @@
         <v>Untitled Document</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>55</v>
       </c>
@@ -2844,7 +2850,7 @@
         <v>C:\temp\</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -2871,13 +2877,13 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="28" customWidth="1"/>
-    <col min="2" max="2" width="80.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="80.5546875" style="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
         <v>111</v>
       </c>
@@ -2885,7 +2891,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
         <v>117</v>
       </c>
@@ -2893,7 +2899,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="28" t="s">
         <v>113</v>
       </c>
@@ -2901,7 +2907,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="28" t="s">
         <v>115</v>
       </c>
@@ -2909,7 +2915,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
         <v>139</v>
       </c>
@@ -2917,12 +2923,12 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" s="27" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" s="27" t="s">
         <v>116</v>
       </c>
@@ -2941,21 +2947,21 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="49" customWidth="1"/>
-    <col min="2" max="2" width="46.140625" style="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" style="44" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.7109375" style="44" customWidth="1"/>
-    <col min="5" max="5" width="50.28515625" style="52" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="52"/>
+    <col min="1" max="1" width="15.6640625" style="49" customWidth="1"/>
+    <col min="2" max="2" width="46.109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="44" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.6640625" style="44" customWidth="1"/>
+    <col min="5" max="5" width="50.33203125" style="52" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="49" t="s">
         <v>105</v>
       </c>
@@ -2964,7 +2970,7 @@
       </c>
       <c r="D1" s="47"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="49" t="s">
         <v>89</v>
       </c>
@@ -2972,7 +2978,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="49" t="s">
         <v>87</v>
       </c>
@@ -2980,7 +2986,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="49" t="s">
         <v>88</v>
       </c>
@@ -2988,7 +2994,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="49" t="s">
         <v>91</v>
       </c>
@@ -2997,12 +3003,12 @@
       </c>
       <c r="D5" s="45"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="50" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="49" t="s">
         <v>105</v>
       </c>
@@ -3011,15 +3017,15 @@
       </c>
       <c r="D8" s="47"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="70" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="49" t="s">
         <v>87</v>
       </c>
@@ -3027,7 +3033,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="49" t="s">
         <v>88</v>
       </c>
@@ -3035,7 +3041,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="49" t="s">
         <v>91</v>
       </c>
@@ -3043,12 +3049,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" s="50" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="49" t="s">
         <v>105</v>
       </c>
@@ -3057,15 +3063,15 @@
       </c>
       <c r="D15" s="47"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="79" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="49" t="s">
         <v>87</v>
       </c>
@@ -3073,7 +3079,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="49" t="s">
         <v>88</v>
       </c>
@@ -3081,7 +3087,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="49" t="s">
         <v>91</v>
       </c>
@@ -3089,12 +3095,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" s="51" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="49" t="s">
         <v>105</v>
       </c>
@@ -3103,7 +3109,7 @@
       </c>
       <c r="D22" s="47"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="49" t="s">
         <v>89</v>
       </c>
@@ -3113,7 +3119,7 @@
       <c r="C23" s="43"/>
       <c r="D23" s="46"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="49" t="s">
         <v>87</v>
       </c>
@@ -3121,7 +3127,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="49" t="s">
         <v>88</v>
       </c>
@@ -3129,7 +3135,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="49" t="s">
         <v>91</v>
       </c>
@@ -3138,12 +3144,12 @@
       </c>
       <c r="D26" s="45"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" s="50" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="49" t="s">
         <v>105</v>
       </c>
@@ -3151,7 +3157,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="49" t="s">
         <v>89</v>
       </c>
@@ -3162,7 +3168,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="49" t="s">
         <v>87</v>
       </c>
@@ -3170,7 +3176,7 @@
         <v>71600223</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="49" t="s">
         <v>88</v>
       </c>
@@ -3178,7 +3184,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="49" t="s">
         <v>91</v>
       </c>
@@ -3186,12 +3192,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B34" s="50" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="49" t="s">
         <v>105</v>
       </c>
@@ -3199,7 +3205,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="49" t="s">
         <v>89</v>
       </c>
@@ -3207,7 +3213,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="49" t="s">
         <v>87</v>
       </c>
@@ -3215,7 +3221,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="49" t="s">
         <v>88</v>
       </c>
@@ -3223,7 +3229,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="49" t="s">
         <v>91</v>
       </c>
@@ -3231,25 +3237,25 @@
         <v>144</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B41" s="50" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B48" s="37"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" s="40"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B16" r:id="rId1" xr:uid="{A65A84B2-71FA-4431-BCFE-09318E51B44B}"/>
-    <hyperlink ref="B30" r:id="rId2" xr:uid="{91A65524-5E97-495A-9570-B1A58E8D5401}"/>
-    <hyperlink ref="C30" r:id="rId3" xr:uid="{EDF48202-E921-4C45-BCE8-6B400B300D47}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{9E2F953D-5EE9-40BD-AF1C-40E5805312FA}"/>
-    <hyperlink ref="B37" r:id="rId5" xr:uid="{4433C870-7E4C-4C18-A923-94FA8AABE4FA}"/>
-    <hyperlink ref="B9" r:id="rId6" xr:uid="{C2B89067-FB4F-4879-9341-F4A481DD774D}"/>
+    <hyperlink ref="B30" r:id="rId1" xr:uid="{91A65524-5E97-495A-9570-B1A58E8D5401}"/>
+    <hyperlink ref="C30" r:id="rId2" xr:uid="{EDF48202-E921-4C45-BCE8-6B400B300D47}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{9E2F953D-5EE9-40BD-AF1C-40E5805312FA}"/>
+    <hyperlink ref="B37" r:id="rId4" xr:uid="{4433C870-7E4C-4C18-A923-94FA8AABE4FA}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{C2B89067-FB4F-4879-9341-F4A481DD774D}"/>
+    <hyperlink ref="B16" r:id="rId6" xr:uid="{A65A84B2-71FA-4431-BCFE-09318E51B44B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -3264,17 +3270,17 @@
       <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="54" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" style="54" customWidth="1"/>
     <col min="2" max="2" width="41" style="60" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="56" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" style="56" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41" style="56" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.28515625" style="58" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="58"/>
+    <col min="5" max="5" width="50.33203125" style="58" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="54" t="s">
         <v>105</v>
       </c>
@@ -3283,7 +3289,7 @@
       </c>
       <c r="D1" s="57"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="54" t="s">
         <v>89</v>
       </c>
@@ -3291,7 +3297,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="54" t="s">
         <v>87</v>
       </c>
@@ -3299,7 +3305,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="54" t="s">
         <v>88</v>
       </c>
@@ -3307,7 +3313,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="54" t="s">
         <v>91</v>
       </c>
@@ -3316,12 +3322,12 @@
       </c>
       <c r="D5" s="61"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="62" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="54" t="s">
         <v>105</v>
       </c>
@@ -3330,7 +3336,7 @@
       </c>
       <c r="D8" s="57"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="54" t="s">
         <v>89</v>
       </c>
@@ -3338,7 +3344,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="54" t="s">
         <v>87</v>
       </c>
@@ -3346,7 +3352,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="54" t="s">
         <v>88</v>
       </c>
@@ -3354,7 +3360,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="54" t="s">
         <v>91</v>
       </c>
@@ -3362,12 +3368,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" s="62" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="54" t="s">
         <v>105</v>
       </c>
@@ -3376,7 +3382,7 @@
       </c>
       <c r="D15" s="57"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="54" t="s">
         <v>89</v>
       </c>
@@ -3384,7 +3390,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="54" t="s">
         <v>87</v>
       </c>
@@ -3392,7 +3398,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="54" t="s">
         <v>88</v>
       </c>
@@ -3400,7 +3406,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="54" t="s">
         <v>91</v>
       </c>
@@ -3408,12 +3414,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" s="65" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="54" t="s">
         <v>105</v>
       </c>
@@ -3422,7 +3428,7 @@
       </c>
       <c r="D22" s="57"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="54" t="s">
         <v>89</v>
       </c>
@@ -3432,7 +3438,7 @@
       <c r="C23" s="66"/>
       <c r="D23" s="67"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="54" t="s">
         <v>87</v>
       </c>
@@ -3440,7 +3446,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="54" t="s">
         <v>88</v>
       </c>
@@ -3448,7 +3454,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="54" t="s">
         <v>91</v>
       </c>
@@ -3457,12 +3463,12 @@
       </c>
       <c r="D26" s="61"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" s="62" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="54" t="s">
         <v>105</v>
       </c>
@@ -3470,7 +3476,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A30" s="54" t="s">
         <v>89</v>
       </c>
@@ -3484,7 +3490,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="54" t="s">
         <v>87</v>
       </c>
@@ -3492,7 +3498,7 @@
         <v>71600223</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="54" t="s">
         <v>88</v>
       </c>
@@ -3500,7 +3506,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="54" t="s">
         <v>91</v>
       </c>
@@ -3508,12 +3514,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B34" s="62" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="54" t="s">
         <v>105</v>
       </c>
@@ -3521,7 +3527,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="54" t="s">
         <v>89</v>
       </c>
@@ -3529,7 +3535,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="54" t="s">
         <v>87</v>
       </c>
@@ -3537,7 +3543,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="54" t="s">
         <v>88</v>
       </c>
@@ -3546,7 +3552,7 @@
       </c>
       <c r="D39" s="61"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="54" t="s">
         <v>91</v>
       </c>
@@ -3554,15 +3560,15 @@
         <v>144</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B41" s="62" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B48" s="55"/>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" s="63"/>
     </row>
   </sheetData>
@@ -3585,114 +3591,114 @@
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="165.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="165.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19"/>
     </row>
-    <row r="2" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="36" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
       <c r="D4" s="16"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>70</v>
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="18"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="18"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="20" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
         <v>74</v>
       </c>

</xml_diff>

<commit_message>
Commit after SIT (20-04-2023)
Commit after SIT (20-04-2023)
</commit_message>
<xml_diff>
--- a/Project_Notebook.xlsx
+++ b/Project_Notebook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SCC-IT\Documents\UiPath\SCC-Kuantan\GitHub\Auto-Generate-LE-Weekly-Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52234FB9-6F73-4070-A4D0-D4BAFC7C552B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E631C2-DABE-4F7C-A16D-5E7266D3EFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9024" firstSheet="1" activeTab="6" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8124" firstSheet="1" activeTab="5" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Scratchpad" sheetId="6" r:id="rId1"/>
@@ -77,7 +77,7 @@
     <definedName name="LE_KT_PWD" localSheetId="7">'Access (2)'!$B$26</definedName>
     <definedName name="LE_KT_PWD">Access!$B$26</definedName>
     <definedName name="LE_KT_URL" localSheetId="7">'Access (2)'!#REF!</definedName>
-    <definedName name="LE_KT_URL">Access!#REF!</definedName>
+    <definedName name="LE_KT_URL">Access!$B$23</definedName>
     <definedName name="LE_KT_USERNAME" localSheetId="7">'Access (2)'!$B$25</definedName>
     <definedName name="LE_KT_USERNAME">Access!$B$25</definedName>
     <definedName name="LE_KU_CREDENTIAL" localSheetId="7">'Access (2)'!$B$6</definedName>
@@ -112,16 +112,17 @@
     <definedName name="LE_PC_URL_LOCAL">Access!#REF!</definedName>
     <definedName name="LE_PC_USERNAME" localSheetId="7">'Access (2)'!$B$32</definedName>
     <definedName name="LE_PC_USERNAME">Access!#REF!</definedName>
+    <definedName name="LE_PRESENTATION_URL">Config!$B$6</definedName>
     <definedName name="LE_SB_CREDENTIAL" localSheetId="7">'Access (2)'!$B$41</definedName>
-    <definedName name="LE_SB_CREDENTIAL">Access!#REF!</definedName>
+    <definedName name="LE_SB_CREDENTIAL">Access!$B$41</definedName>
     <definedName name="LE_SB_ID" localSheetId="7">'Access (2)'!$B$38</definedName>
-    <definedName name="LE_SB_ID">Access!#REF!</definedName>
+    <definedName name="LE_SB_ID">Access!$B$38</definedName>
     <definedName name="LE_SB_PWD" localSheetId="7">'Access (2)'!$B$40</definedName>
-    <definedName name="LE_SB_PWD">Access!#REF!</definedName>
+    <definedName name="LE_SB_PWD">Access!$B$40</definedName>
     <definedName name="LE_SB_URL" localSheetId="7">'Access (2)'!$B$37</definedName>
-    <definedName name="LE_SB_URL">Access!#REF!</definedName>
+    <definedName name="LE_SB_URL">Access!$B$37</definedName>
     <definedName name="LE_SB_USERNAME" localSheetId="7">'Access (2)'!$B$39</definedName>
-    <definedName name="LE_SB_USERNAME">Access!#REF!</definedName>
+    <definedName name="LE_SB_USERNAME">Access!$B$39</definedName>
     <definedName name="Length">Text!$B$6</definedName>
     <definedName name="LowerCase">Text!$B$8</definedName>
     <definedName name="MK" localSheetId="7">'Access (2)'!$B$8</definedName>
@@ -140,6 +141,7 @@
     <definedName name="Report_Folder">Config!$B$2</definedName>
     <definedName name="Report_Sub_URL">Config!$B$5</definedName>
     <definedName name="Result">Text!$B$12</definedName>
+    <definedName name="SB">Access!$B$36</definedName>
     <definedName name="Search">Text!$B$10</definedName>
     <definedName name="Text_Input">Text!$B$4</definedName>
     <definedName name="ThisMonthFirstWorkingDay">Date!$B$16</definedName>
@@ -169,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="147">
   <si>
     <t>Last month's dates (First and Last)</t>
   </si>
@@ -606,6 +608,12 @@
   </si>
   <si>
     <t>it1234</t>
+  </si>
+  <si>
+    <t>setup/presentation/indexPage.aspx</t>
+  </si>
+  <si>
+    <t>Presentation URL</t>
   </si>
 </sst>
 </file>
@@ -1374,6 +1382,9 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1397,9 +1408,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -1996,20 +2004,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
     </row>
     <row r="2" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="78" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -2020,7 +2028,7 @@
       </c>
       <c r="B4" s="29">
         <f ca="1">TODAY()</f>
-        <v>45028</v>
+        <v>45036</v>
       </c>
       <c r="C4" s="26">
         <v>5</v>
@@ -2048,7 +2056,7 @@
       </c>
       <c r="B8" s="29" t="str">
         <f ca="1">TEXT(Date_Input+Days, preferred_date_format)</f>
-        <v>07/04/2023</v>
+        <v>15/04/2023</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -2057,7 +2065,7 @@
       </c>
       <c r="B9" s="29" t="str">
         <f ca="1">TEXT(WORKDAY(Date_Input, Days),preferred_date_format)</f>
-        <v>05/04/2023</v>
+        <v>13/04/2023</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -2066,7 +2074,7 @@
       </c>
       <c r="B10" s="26" t="str">
         <f ca="1">TEXT(Date_Input,"YYYYMMDD")</f>
-        <v>20230412</v>
+        <v>20230420</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -2075,7 +2083,7 @@
       </c>
       <c r="B12" s="29" t="str">
         <f ca="1">TEXT(TODAY(), preferred_date_format)</f>
-        <v>12/04/2023</v>
+        <v>20/04/2023</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -2084,31 +2092,31 @@
       </c>
       <c r="B13" s="29" t="str">
         <f ca="1">TEXT(TODAY()-6, preferred_date_format)</f>
-        <v>06/04/2023</v>
+        <v>14/04/2023</v>
       </c>
       <c r="C13" s="29" t="str">
         <f ca="1">TEXT(TODAY()-5, preferred_date_format)</f>
-        <v>07/04/2023</v>
+        <v>15/04/2023</v>
       </c>
       <c r="D13" s="29" t="str">
         <f ca="1">TEXT(TODAY()-4, preferred_date_format)</f>
-        <v>08/04/2023</v>
+        <v>16/04/2023</v>
       </c>
       <c r="E13" s="29" t="str">
         <f ca="1">TEXT(TODAY()-3, preferred_date_format)</f>
-        <v>09/04/2023</v>
+        <v>17/04/2023</v>
       </c>
       <c r="F13" s="29" t="str">
         <f ca="1">TEXT(TODAY()-2, preferred_date_format)</f>
-        <v>10/04/2023</v>
+        <v>18/04/2023</v>
       </c>
       <c r="G13" s="29" t="str">
         <f ca="1">TEXT(TODAY()-1, preferred_date_format)</f>
-        <v>11/04/2023</v>
+        <v>19/04/2023</v>
       </c>
       <c r="H13" s="29" t="str">
         <f ca="1">TEXT(TODAY(), preferred_date_format)</f>
-        <v>12/04/2023</v>
+        <v>20/04/2023</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -2117,31 +2125,31 @@
       </c>
       <c r="B14" s="29" t="str">
         <f ca="1">TEXT(TODAY()-WEEKDAY(TODAY(),2)-6, preferred_date_format)</f>
-        <v>03/04/2023</v>
+        <v>10/04/2023</v>
       </c>
       <c r="C14" s="29" t="str">
         <f ca="1">TEXT(TODAY()-WEEKDAY(TODAY(),2)-5, preferred_date_format)</f>
-        <v>04/04/2023</v>
+        <v>11/04/2023</v>
       </c>
       <c r="D14" s="29" t="str">
         <f ca="1">TEXT(TODAY()-WEEKDAY(TODAY(),2)-4, preferred_date_format)</f>
-        <v>05/04/2023</v>
+        <v>12/04/2023</v>
       </c>
       <c r="E14" s="29" t="str">
         <f ca="1">TEXT(TODAY()-WEEKDAY(TODAY(),2)-3, preferred_date_format)</f>
-        <v>06/04/2023</v>
+        <v>13/04/2023</v>
       </c>
       <c r="F14" s="29" t="str">
         <f ca="1">TEXT(TODAY()-WEEKDAY(TODAY(),2)-2, preferred_date_format)</f>
-        <v>07/04/2023</v>
+        <v>14/04/2023</v>
       </c>
       <c r="G14" s="29" t="str">
         <f ca="1">TEXT(TODAY()-WEEKDAY(TODAY(),2)-1, preferred_date_format)</f>
-        <v>08/04/2023</v>
+        <v>15/04/2023</v>
       </c>
       <c r="H14" s="29" t="str">
         <f ca="1">TEXT(TODAY()-WEEKDAY(TODAY(),2), preferred_date_format)</f>
-        <v>09/04/2023</v>
+        <v>16/04/2023</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -2191,11 +2199,11 @@
       </c>
       <c r="B19" s="29" t="str">
         <f ca="1">TEXT(TODAY()-6, preferred_date_format)</f>
-        <v>06/04/2023</v>
+        <v>14/04/2023</v>
       </c>
       <c r="C19" s="29" t="str">
         <f ca="1">TEXT(TODAY()-8, preferred_date_format)</f>
-        <v>04/04/2023</v>
+        <v>12/04/2023</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -2204,11 +2212,11 @@
       </c>
       <c r="B20" s="29" t="str">
         <f ca="1">TEXT(TODAY()-2, preferred_date_format)</f>
-        <v>10/04/2023</v>
+        <v>18/04/2023</v>
       </c>
       <c r="C20" s="29" t="str">
         <f ca="1">TEXT(TODAY()-4, preferred_date_format)</f>
-        <v>08/04/2023</v>
+        <v>16/04/2023</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2217,12 +2225,12 @@
     </row>
     <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="73" t="s">
+      <c r="A23" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="75"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="76"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
@@ -2234,11 +2242,11 @@
       <c r="A25" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="71" t="s">
+      <c r="B25" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="71"/>
-      <c r="D25" s="72"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="73"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
@@ -2397,24 +2405,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="78" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -2631,18 +2639,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="76"/>
+      <c r="B1" s="77"/>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="77"/>
+      <c r="B2" s="78"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
     </row>
@@ -2689,10 +2697,10 @@
     </row>
     <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="75"/>
+      <c r="B9" s="76"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
@@ -2767,18 +2775,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="76"/>
+      <c r="B1" s="77"/>
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="78" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="77"/>
+      <c r="B2" s="78"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
     </row>
@@ -2789,10 +2797,10 @@
       <c r="D3" s="23"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="75"/>
+      <c r="B4" s="76"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
@@ -2873,8 +2881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D25349-4B39-4221-90B0-AC4514B6ED0A}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2921,6 +2929,14 @@
       </c>
       <c r="B5" s="27" t="s">
         <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -2947,8 +2963,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3067,7 +3083,7 @@
       <c r="A16" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="79" t="s">
+      <c r="B16" s="71" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>